<commit_message>
Update example device list
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>Resource Registry Init</t>
   </si>
@@ -148,6 +148,27 @@
   </si>
   <si>
     <t>7fd248f5-e698-46f1-b30e-1ac568d66c15</t>
+  </si>
+  <si>
+    <t>connection-type</t>
+  </si>
+  <si>
+    <t>ssh</t>
+  </si>
+  <si>
+    <t>shh</t>
+  </si>
+  <si>
+    <t>connection-port</t>
+  </si>
+  <si>
+    <t>DC_Shell</t>
+  </si>
+  <si>
+    <t>DC_Dummy</t>
+  </si>
+  <si>
+    <t>DC_Dummy2</t>
   </si>
 </sst>
 </file>
@@ -216,7 +237,98 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -230,9 +342,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TDEVICES" displayName="TDEVICES" ref="A1:Q15" totalsRowShown="0">
-  <autoFilter ref="A1:Q15"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TDEVICES" displayName="TDEVICES" ref="A1:V15" totalsRowShown="0">
+  <autoFilter ref="A1:V15"/>
+  <tableColumns count="22">
     <tableColumn id="1" name="Device"/>
     <tableColumn id="2" name="OS"/>
     <tableColumn id="3" name="user"/>
@@ -246,6 +358,11 @@
     <tableColumn id="11" name="eth1 IP"/>
     <tableColumn id="12" name="is_resource"/>
     <tableColumn id="13" name="UUID"/>
+    <tableColumn id="14" name="connection-type" dataDxfId="4"/>
+    <tableColumn id="19" name="connection-port" dataDxfId="3"/>
+    <tableColumn id="20" name="DC_Dummy" dataDxfId="2"/>
+    <tableColumn id="21" name="DC_Shell" dataDxfId="1"/>
+    <tableColumn id="22" name="DC_Dummy2" dataDxfId="0"/>
     <tableColumn id="15" name="DC_Docker"/>
     <tableColumn id="16" name="DC_Transferapp"/>
     <tableColumn id="17" name="DC_Swarm"/>
@@ -661,10 +778,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -682,14 +799,19 @@
     <col min="11" max="11" width="14.44140625" style="2" customWidth="1"/>
     <col min="12" max="12" width="12.5546875" style="3" customWidth="1"/>
     <col min="13" max="13" width="36" style="3" customWidth="1"/>
-    <col min="14" max="14" width="12.44140625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="16.5546875" style="3" customWidth="1"/>
-    <col min="16" max="16" width="12.109375" style="3" customWidth="1"/>
-    <col min="17" max="17" width="9.44140625" style="3" customWidth="1"/>
-    <col min="1021" max="1023" width="9.109375" customWidth="1"/>
+    <col min="14" max="14" width="14.44140625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="17.77734375" style="3" customWidth="1"/>
+    <col min="16" max="16" width="36" style="3" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="14.44140625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="12.44140625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="16.5546875" style="3" customWidth="1"/>
+    <col min="21" max="21" width="12.109375" style="3" customWidth="1"/>
+    <col min="22" max="22" width="9.44140625" style="3" customWidth="1"/>
+    <col min="1026" max="1028" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -730,19 +852,34 @@
         <v>16</v>
       </c>
       <c r="N1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="S1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
@@ -779,19 +916,32 @@
         <v>31</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>27</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="O2" s="5">
+        <v>22</v>
+      </c>
+      <c r="P2" s="5"/>
       <c r="Q2" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
@@ -826,19 +976,32 @@
         <v>40</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>27</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="O3" s="5">
+        <v>22</v>
+      </c>
+      <c r="P3" s="5"/>
       <c r="Q3" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -856,8 +1019,13 @@
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
-    </row>
-    <row r="5" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+    </row>
+    <row r="5" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -875,8 +1043,13 @@
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
-    </row>
-    <row r="6" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+    </row>
+    <row r="6" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -894,8 +1067,13 @@
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
-    </row>
-    <row r="7" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+    </row>
+    <row r="7" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -913,8 +1091,13 @@
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
-    </row>
-    <row r="8" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+    </row>
+    <row r="8" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -932,8 +1115,13 @@
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
-    </row>
-    <row r="9" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+    </row>
+    <row r="9" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -951,8 +1139,13 @@
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
-    </row>
-    <row r="10" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+    </row>
+    <row r="10" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -970,8 +1163,13 @@
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
-    </row>
-    <row r="11" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+    </row>
+    <row r="11" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -989,8 +1187,13 @@
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
-    </row>
-    <row r="12" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+    </row>
+    <row r="12" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1008,8 +1211,13 @@
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
-    </row>
-    <row r="13" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+    </row>
+    <row r="13" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1027,8 +1235,13 @@
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
-    </row>
-    <row r="14" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+    </row>
+    <row r="14" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -1046,8 +1259,13 @@
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
-    </row>
-    <row r="15" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+    </row>
+    <row r="15" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1065,8 +1283,13 @@
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
-    </row>
-    <row r="16" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+    </row>
+    <row r="16" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>

</xml_diff>